<commit_message>
Saving results previous to update
</commit_message>
<xml_diff>
--- a/data/tables/paradigms.xlsx
+++ b/data/tables/paradigms.xlsx
@@ -1,86 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\TsakonianDB\data\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\tsakonian_dictionary_app\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DFB3A5-C324-4E6A-B7C6-D2484F6302F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA7A927-F791-43C4-BE79-C357CD9F42E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="139">
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>ο, pl. -οι</t>
-  </si>
-  <si>
     <t>A5</t>
   </si>
   <si>
-    <t>ο, pl. -ε</t>
-  </si>
-  <si>
-    <t>ο, pl. -ου</t>
-  </si>
-  <si>
-    <t>ο, pl. -δε</t>
-  </si>
-  <si>
-    <t>ο, pl. -ουνε</t>
-  </si>
-  <si>
-    <t>α, pl. -ε</t>
-  </si>
-  <si>
-    <t>α, pl. -λε</t>
-  </si>
-  <si>
-    <t>α, pl. -αδε</t>
-  </si>
-  <si>
-    <t>α, pl. -ουδε</t>
-  </si>
-  <si>
-    <t>α, pl. irregular</t>
-  </si>
-  <si>
-    <t>το, pl. -ματα</t>
-  </si>
-  <si>
-    <t>το, pl. -α</t>
-  </si>
-  <si>
-    <t>το, pl. -ητα</t>
-  </si>
-  <si>
-    <t>το, pl. -ατα</t>
-  </si>
-  <si>
-    <t>το, pl. irregular</t>
-  </si>
-  <si>
-    <t>ο, pl. irregular</t>
-  </si>
-  <si>
     <t>-ε, -α, -ε</t>
   </si>
   <si>
@@ -171,9 +134,6 @@
     <t>Υ5</t>
   </si>
   <si>
-    <t>το, pl. -ια</t>
-  </si>
-  <si>
     <t>Α</t>
   </si>
   <si>
@@ -219,54 +179,6 @@
     <t>Α6</t>
   </si>
   <si>
-    <t>ου</t>
-  </si>
-  <si>
-    <t>ε</t>
-  </si>
-  <si>
-    <t>λε</t>
-  </si>
-  <si>
-    <t>αδε</t>
-  </si>
-  <si>
-    <t>ουδε</t>
-  </si>
-  <si>
-    <t>ματα</t>
-  </si>
-  <si>
-    <t>ια</t>
-  </si>
-  <si>
-    <t>ητα</t>
-  </si>
-  <si>
-    <t>ατα</t>
-  </si>
-  <si>
-    <t>οι</t>
-  </si>
-  <si>
-    <t>ουνε</t>
-  </si>
-  <si>
-    <t>δε</t>
-  </si>
-  <si>
-    <t>άε</t>
-  </si>
-  <si>
-    <t>α, pl. -άε</t>
-  </si>
-  <si>
-    <t>μάτου</t>
-  </si>
-  <si>
-    <t>ίου</t>
-  </si>
-  <si>
     <t>γέρου</t>
   </si>
   <si>
@@ -376,6 +288,171 @@
   </si>
   <si>
     <t>υβάτου</t>
+  </si>
+  <si>
+    <t>ο, πλ. -οι</t>
+  </si>
+  <si>
+    <t>ο, πλ. -ε</t>
+  </si>
+  <si>
+    <t>ο, πλ. -ου</t>
+  </si>
+  <si>
+    <t>ο, πλ. -δε</t>
+  </si>
+  <si>
+    <t>α, πλ. -ε</t>
+  </si>
+  <si>
+    <t>α, πλ. -λε</t>
+  </si>
+  <si>
+    <t>α, πλ. -άε</t>
+  </si>
+  <si>
+    <t>α, πλ. -αδε</t>
+  </si>
+  <si>
+    <t>α, πλ. -ουδε</t>
+  </si>
+  <si>
+    <t>το, πλ. -ητα</t>
+  </si>
+  <si>
+    <t>το, πλ. -ατα</t>
+  </si>
+  <si>
+    <t>-οι</t>
+  </si>
+  <si>
+    <t>-ε</t>
+  </si>
+  <si>
+    <t>-ου</t>
+  </si>
+  <si>
+    <t>-ουνε</t>
+  </si>
+  <si>
+    <t>-δε</t>
+  </si>
+  <si>
+    <t>-λε</t>
+  </si>
+  <si>
+    <t>-άε</t>
+  </si>
+  <si>
+    <t>-αδε</t>
+  </si>
+  <si>
+    <t>-ουδε</t>
+  </si>
+  <si>
+    <t>-α</t>
+  </si>
+  <si>
+    <t>-ματα</t>
+  </si>
+  <si>
+    <t>-ια</t>
+  </si>
+  <si>
+    <t>-ητα</t>
+  </si>
+  <si>
+    <t>-ατα</t>
+  </si>
+  <si>
+    <t>-ίου</t>
+  </si>
+  <si>
+    <t>-μάτου</t>
+  </si>
+  <si>
+    <t>ο, πλ. αθήνε</t>
+  </si>
+  <si>
+    <t>o, πλ. γέροι</t>
+  </si>
+  <si>
+    <t>ο, πλ. ουθίουνε</t>
+  </si>
+  <si>
+    <t>α, πλ. κρόπε</t>
+  </si>
+  <si>
+    <t>το, πλ. κόκα</t>
+  </si>
+  <si>
+    <t>το, πλ. τσ̌έρβα</t>
+  </si>
+  <si>
+    <t>το, πλ. π̇ιτόκα</t>
+  </si>
+  <si>
+    <t>το, πλ. κάβα</t>
+  </si>
+  <si>
+    <t>το, πλ. μάβα</t>
+  </si>
+  <si>
+    <t>το, πλ. άζα</t>
+  </si>
+  <si>
+    <t>ο, πλ. ψιλ̣οί, γεν. ψιού</t>
+  </si>
+  <si>
+    <t>ο, πλ. κούν̇οι, γεν. κουνέ</t>
+  </si>
+  <si>
+    <t>α, πλ. σατέρε, γεν. σάτη / σατερί</t>
+  </si>
+  <si>
+    <t>α, πλ. ματέρε, γεν. μάτη / ματερί</t>
+  </si>
+  <si>
+    <t>α, πλ. άμπελε, γεν. άμπελε / άμπελ̣ή</t>
+  </si>
+  <si>
+    <t>το, πλ. ύβατα, γεν. υβάτου</t>
+  </si>
+  <si>
+    <t>ο, πλ. ανόμαλος</t>
+  </si>
+  <si>
+    <t>α, πλ. ανόμαλος</t>
+  </si>
+  <si>
+    <t>το, πλ. ανόμαλος</t>
+  </si>
+  <si>
+    <t>ο, πλ. -ουνε, γεν. -ου</t>
+  </si>
+  <si>
+    <t>ο, πλ. -ου, γεν. -ου</t>
+  </si>
+  <si>
+    <t>το, πλ. -α, γεν. -ου</t>
+  </si>
+  <si>
+    <t>το, πλ. -ματα, γεν. -μάτου</t>
+  </si>
+  <si>
+    <t>το, πλ. -ια, γεν. -ίου</t>
+  </si>
+  <si>
+    <t>Ρ</t>
+  </si>
+  <si>
+    <t>ρήμα</t>
+  </si>
+  <si>
+    <t>Ε</t>
+  </si>
+  <si>
+    <t>επίθ.</t>
   </si>
 </sst>
 </file>
@@ -531,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}" name="Tabla2" displayName="Tabla2" ref="A1:D48" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D48" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}" name="Tabla2" displayName="Tabla2" ref="A1:D50" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D50" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C1DD779A-CDEE-46F1-B76C-117DD684DD75}" name="paradigm" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{4C03C951-46D8-47E8-8244-B52757673F4E}" name="notes" dataDxfId="2"/>
@@ -806,554 +883,607 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>73</v>
+      <c r="D3" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>65</v>
+      <c r="D4" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>64</v>
+      <c r="D5" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>130</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>75</v>
+      <c r="D7" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>64</v>
+        <v>131</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>65</v>
+      <c r="D10" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>66</v>
+      <c r="D11" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>76</v>
+      <c r="D12" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>67</v>
+      <c r="D13" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
+      <c r="D14" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>132</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>133</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>134</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>71</v>
+      <c r="D19" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
+      <c r="D20" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="C38" s="1" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C39" s="1" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="C40" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D41" s="1" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="D42" s="1" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>115</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>